<commit_message>
updated values with latest run
</commit_message>
<xml_diff>
--- a/data/SuperEndpoint Mapping 2021NOV04.xlsx
+++ b/data/SuperEndpoint Mapping 2021NOV04.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://pnnl-my.sharepoint.com/personal/sara_gosline_pnnl_gov/Documents/Documents/GitHub/srpAnalytics/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="13" documentId="13_ncr:1_{ACEAD2CE-F3FB-441B-BA99-37A330197109}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FC5F8F51-6F23-4C1E-A63A-3187D3680CA0}"/>
+  <xr:revisionPtr revIDLastSave="16" documentId="13_ncr:1_{ACEAD2CE-F3FB-441B-BA99-37A330197109}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A5CAD3E4-EDFA-4BC3-B8C2-FE389EA3110F}"/>
   <bookViews>
-    <workbookView xWindow="31500" yWindow="780" windowWidth="21600" windowHeight="12735" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13785" yWindow="2880" windowWidth="21600" windowHeight="12735" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Original" sheetId="4" r:id="rId1"/>
@@ -208,9 +208,6 @@
     <t>TOT_MORT</t>
   </si>
   <si>
-    <t>ANY_MORT</t>
-  </si>
-  <si>
     <t>BRN_    </t>
   </si>
   <si>
@@ -220,9 +217,6 @@
     <t>EDEM    </t>
   </si>
   <si>
-    <t>LTKR    </t>
-  </si>
-  <si>
     <t>MUSC    </t>
   </si>
   <si>
@@ -665,6 +659,12 @@
   </si>
   <si>
     <t>http://purl.obolibrary.org/obo/ZP_0015467</t>
+  </si>
+  <si>
+    <t>ALL_BUT_MORT</t>
+  </si>
+  <si>
+    <t>NC__</t>
   </si>
 </sst>
 </file>
@@ -791,10 +791,10 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1160,13 +1160,13 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F1" t="s">
         <v>80</v>
-      </c>
-      <c r="C1" t="s">
-        <v>69</v>
-      </c>
-      <c r="F1" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -1174,10 +1174,10 @@
         <v>7</v>
       </c>
       <c r="B2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C2" t="s">
         <v>79</v>
-      </c>
-      <c r="C2" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -1185,10 +1185,10 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -1196,10 +1196,10 @@
         <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C4" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -1207,21 +1207,21 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C5" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B6" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C6" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -1229,21 +1229,21 @@
         <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C7" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B8" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C8" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -1251,10 +1251,10 @@
         <v>26</v>
       </c>
       <c r="B9" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C9" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -1262,43 +1262,43 @@
         <v>29</v>
       </c>
       <c r="B10" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C10" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B11" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C11" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B12" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C12" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B13" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C13" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -1306,10 +1306,10 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C14" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -1317,43 +1317,43 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C15" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B16" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C16" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B17" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C17" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B18" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C18" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -1361,43 +1361,43 @@
         <v>30</v>
       </c>
       <c r="B19" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C19" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B20" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C20" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B21" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C21" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B22" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C22" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
   </sheetData>
@@ -1431,11 +1431,11 @@
       <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -1718,7 +1718,7 @@
   <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1730,83 +1730,83 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E1" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>59</v>
+        <v>210</v>
       </c>
       <c r="C2" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>57</v>
       </c>
       <c r="C3" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B4" s="8" t="s">
         <v>56</v>
       </c>
       <c r="C4" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>74</v>
-      </c>
-      <c r="E5" s="14" t="s">
-        <v>198</v>
+        <v>72</v>
+      </c>
+      <c r="E5" s="13" t="s">
+        <v>196</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B6" s="8" t="s">
         <v>9</v>
@@ -1815,248 +1815,248 @@
         <v>8</v>
       </c>
       <c r="D6" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="E6" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C7" t="s">
         <v>10</v>
       </c>
       <c r="D7" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="E7" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C8" t="s">
         <v>14</v>
       </c>
       <c r="D8" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="E8" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B9" s="10" t="s">
         <v>4</v>
       </c>
       <c r="C9" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="E9" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C10" t="s">
         <v>19</v>
       </c>
       <c r="D10" t="s">
-        <v>176</v>
-      </c>
-      <c r="E10" s="14" t="s">
-        <v>203</v>
+        <v>174</v>
+      </c>
+      <c r="E10" s="13" t="s">
+        <v>201</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>63</v>
+        <v>24</v>
       </c>
       <c r="C11" t="s">
         <v>23</v>
       </c>
       <c r="D11" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="E11" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B12" s="8" t="s">
         <v>3</v>
       </c>
       <c r="C12" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D12" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="E12" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B13" s="10" t="s">
         <v>7</v>
       </c>
       <c r="C13" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="D13" s="12" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="E13" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D14" s="12" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E14" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C15" t="s">
         <v>27</v>
       </c>
       <c r="D15" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="E15" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>39</v>
+        <v>211</v>
       </c>
       <c r="C16" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D16" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E16" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C17" t="s">
         <v>32</v>
       </c>
       <c r="D17" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="E17" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B18" s="10" t="s">
         <v>5</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D18" s="11" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="E18" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C19" t="s">
         <v>35</v>
       </c>
       <c r="D19" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="E19" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B20" s="8" t="s">
         <v>58</v>
       </c>
       <c r="C20" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D20" s="9" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E20" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
   </sheetData>
@@ -2091,35 +2091,35 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C2" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B3" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C3" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -2127,10 +2127,10 @@
         <v>26</v>
       </c>
       <c r="B4" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C4" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -2138,43 +2138,43 @@
         <v>29</v>
       </c>
       <c r="B5" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C5" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B6" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C6" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C7" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B8" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C8" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -2182,7 +2182,7 @@
         <v>12</v>
       </c>
       <c r="B9" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -2190,43 +2190,43 @@
         <v>13</v>
       </c>
       <c r="B10" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C10" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B11" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C11" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B12" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C12" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B13" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C13" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -2234,52 +2234,52 @@
         <v>30</v>
       </c>
       <c r="B14" t="s">
+        <v>146</v>
+      </c>
+      <c r="C14" t="s">
+        <v>147</v>
+      </c>
+      <c r="E14" t="s">
         <v>148</v>
       </c>
-      <c r="C14" t="s">
+      <c r="F14" t="s">
         <v>149</v>
       </c>
-      <c r="E14" t="s">
+      <c r="G14" t="s">
         <v>150</v>
-      </c>
-      <c r="F14" t="s">
-        <v>151</v>
-      </c>
-      <c r="G14" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B15" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C15" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B16" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C16" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B17" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C17" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -2287,38 +2287,38 @@
         <v>39</v>
       </c>
       <c r="B18" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C18" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>154</v>
+      </c>
+      <c r="B19" t="s">
+        <v>155</v>
+      </c>
+      <c r="C19" t="s">
         <v>156</v>
       </c>
-      <c r="B19" t="s">
-        <v>157</v>
-      </c>
-      <c r="C19" t="s">
-        <v>158</v>
-      </c>
       <c r="E19" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B20" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C20" t="s">
+        <v>158</v>
+      </c>
+      <c r="E20" t="s">
         <v>160</v>
-      </c>
-      <c r="E20" t="s">
-        <v>162</v>
       </c>
     </row>
   </sheetData>
@@ -2327,6 +2327,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100396ED2E7A640164CB8C59FDEC2C765CC" ma:contentTypeVersion="8" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="26e8590940edae28bea0b080f6fa8b06">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="aceb4bc4-7be6-4130-8e8a-7008d72bfcc3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7a9331905dac936d9e88b896f6b901d6" ns3:_="">
     <xsd:import namespace="aceb4bc4-7be6-4130-8e8a-7008d72bfcc3"/>
@@ -2496,35 +2511,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E8D080FC-E009-4447-ACD6-B9CB0ED3D7DD}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{49E57FCB-AF0B-40B5-9F88-8BBFA3B90FEE}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="aceb4bc4-7be6-4130-8e8a-7008d72bfcc3"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2546,9 +2536,19 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{49E57FCB-AF0B-40B5-9F88-8BBFA3B90FEE}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E8D080FC-E009-4447-ACD6-B9CB0ED3D7DD}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="aceb4bc4-7be6-4130-8e8a-7008d72bfcc3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
updated metadata and mapping
updated chemicals and endpoints
</commit_message>
<xml_diff>
--- a/data/SuperEndpoint Mapping 2021NOV04.xlsx
+++ b/data/SuperEndpoint Mapping 2021NOV04.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://pnnl-my.sharepoint.com/personal/sara_gosline_pnnl_gov/Documents/Documents/GitHub/srpAnalytics/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="16" documentId="13_ncr:1_{ACEAD2CE-F3FB-441B-BA99-37A330197109}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A5CAD3E4-EDFA-4BC3-B8C2-FE389EA3110F}"/>
+  <xr:revisionPtr revIDLastSave="20" documentId="13_ncr:1_{ACEAD2CE-F3FB-441B-BA99-37A330197109}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9F42805B-E5AC-4B5D-8F00-21E7BDD88949}"/>
   <bookViews>
-    <workbookView xWindow="13785" yWindow="2880" windowWidth="21600" windowHeight="12735" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="31845" yWindow="1125" windowWidth="21600" windowHeight="12735" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Original" sheetId="4" r:id="rId1"/>
@@ -244,9 +244,6 @@
     <t>Simple name (&lt;20char)</t>
   </si>
   <si>
-    <t>Behavior-transition from light to dark</t>
-  </si>
-  <si>
     <t>Behavior-total movement in dark minus total movement in light</t>
   </si>
   <si>
@@ -259,9 +256,6 @@
     <t>Any abnormality or death within 5 days (combination of all measurements at 24hr and 5 days)</t>
   </si>
   <si>
-    <t>Any morphological abnormality not including mortality (#2 minus MO24 and MORT)</t>
-  </si>
-  <si>
     <t>120hr mortality</t>
   </si>
   <si>
@@ -589,9 +583,6 @@
     <t>Any effect except mortality</t>
   </si>
   <si>
-    <t>Any effect in 5 days</t>
-  </si>
-  <si>
     <t>Any effect in 24 hours</t>
   </si>
   <si>
@@ -601,9 +592,6 @@
     <t>Delayed development at 24h</t>
   </si>
   <si>
-    <t>5 day behavior transition</t>
-  </si>
-  <si>
     <t>Notochord at 5 days</t>
   </si>
   <si>
@@ -665,6 +653,18 @@
   </si>
   <si>
     <t>NC__</t>
+  </si>
+  <si>
+    <t>Any morphological abnormality not including mortality (ANY120 minus MO24 and MORT)</t>
+  </si>
+  <si>
+    <t>Any effect</t>
+  </si>
+  <si>
+    <t>Behavior transition</t>
+  </si>
+  <si>
+    <t>Behavior-transition from light to dark in 5 days</t>
   </si>
 </sst>
 </file>
@@ -1160,13 +1160,13 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C1" t="s">
         <v>67</v>
       </c>
       <c r="F1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -1174,10 +1174,10 @@
         <v>7</v>
       </c>
       <c r="B2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C2" t="s">
         <v>77</v>
-      </c>
-      <c r="C2" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -1185,10 +1185,10 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -1196,10 +1196,10 @@
         <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C4" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -1207,21 +1207,21 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C5" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B6" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C6" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -1229,21 +1229,21 @@
         <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C7" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B8" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C8" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -1251,10 +1251,10 @@
         <v>26</v>
       </c>
       <c r="B9" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C9" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -1262,43 +1262,43 @@
         <v>29</v>
       </c>
       <c r="B10" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C10" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B11" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C11" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B12" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C12" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B13" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C13" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -1306,10 +1306,10 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C14" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -1317,43 +1317,43 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C15" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B16" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C16" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B17" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C17" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B18" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C18" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -1361,43 +1361,43 @@
         <v>30</v>
       </c>
       <c r="B19" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C19" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B20" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C20" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B21" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C21" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B22" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C22" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
   </sheetData>
@@ -1718,7 +1718,7 @@
   <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1730,7 +1730,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -1742,71 +1742,71 @@
         <v>67</v>
       </c>
       <c r="E1" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="C2" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>76</v>
+        <v>208</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>57</v>
       </c>
       <c r="C3" t="s">
-        <v>186</v>
+        <v>209</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B4" s="8" t="s">
         <v>56</v>
       </c>
       <c r="C4" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B5" s="10" t="s">
         <v>66</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E5" s="13" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B6" s="8" t="s">
         <v>9</v>
@@ -1815,15 +1815,15 @@
         <v>8</v>
       </c>
       <c r="D6" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="E6" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B7" s="8" t="s">
         <v>59</v>
@@ -1832,15 +1832,15 @@
         <v>10</v>
       </c>
       <c r="D7" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="E7" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B8" s="8" t="s">
         <v>60</v>
@@ -1849,32 +1849,32 @@
         <v>14</v>
       </c>
       <c r="D8" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="E8" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B9" s="10" t="s">
         <v>4</v>
       </c>
       <c r="C9" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E9" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B10" s="8" t="s">
         <v>61</v>
@@ -1883,15 +1883,15 @@
         <v>19</v>
       </c>
       <c r="D10" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="E10" s="13" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B11" s="8" t="s">
         <v>24</v>
@@ -1900,66 +1900,66 @@
         <v>23</v>
       </c>
       <c r="D11" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="E11" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B12" s="8" t="s">
         <v>3</v>
       </c>
       <c r="C12" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="D12" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="E12" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B13" s="10" t="s">
         <v>7</v>
       </c>
       <c r="C13" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="D13" s="12" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="E13" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B14" s="10" t="s">
         <v>65</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>190</v>
+        <v>210</v>
       </c>
       <c r="D14" s="12" t="s">
-        <v>71</v>
+        <v>211</v>
       </c>
       <c r="E14" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B15" s="8" t="s">
         <v>62</v>
@@ -1968,32 +1968,32 @@
         <v>27</v>
       </c>
       <c r="D15" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="E15" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="C16" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="D16" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="E16" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B17" s="8" t="s">
         <v>63</v>
@@ -2002,32 +2002,32 @@
         <v>32</v>
       </c>
       <c r="D17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="E17" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B18" s="10" t="s">
         <v>5</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="D18" s="11" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="E18" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B19" s="8" t="s">
         <v>64</v>
@@ -2036,15 +2036,15 @@
         <v>35</v>
       </c>
       <c r="D19" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="E19" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B20" s="8" t="s">
         <v>58</v>
@@ -2056,7 +2056,7 @@
         <v>69</v>
       </c>
       <c r="E20" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
     </row>
   </sheetData>
@@ -2091,35 +2091,35 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C1" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B3" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -2127,10 +2127,10 @@
         <v>26</v>
       </c>
       <c r="B4" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C4" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -2138,43 +2138,43 @@
         <v>29</v>
       </c>
       <c r="B5" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C5" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B6" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C6" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B7" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C7" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B8" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C8" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -2182,7 +2182,7 @@
         <v>12</v>
       </c>
       <c r="B9" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -2190,43 +2190,43 @@
         <v>13</v>
       </c>
       <c r="B10" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C10" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B11" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C11" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B12" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C12" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B13" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C13" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -2234,52 +2234,52 @@
         <v>30</v>
       </c>
       <c r="B14" t="s">
+        <v>144</v>
+      </c>
+      <c r="C14" t="s">
+        <v>145</v>
+      </c>
+      <c r="E14" t="s">
         <v>146</v>
       </c>
-      <c r="C14" t="s">
+      <c r="F14" t="s">
         <v>147</v>
       </c>
-      <c r="E14" t="s">
+      <c r="G14" t="s">
         <v>148</v>
-      </c>
-      <c r="F14" t="s">
-        <v>149</v>
-      </c>
-      <c r="G14" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B15" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C15" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B16" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C16" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B17" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C17" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -2287,38 +2287,38 @@
         <v>39</v>
       </c>
       <c r="B18" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C18" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>152</v>
+      </c>
+      <c r="B19" t="s">
+        <v>153</v>
+      </c>
+      <c r="C19" t="s">
         <v>154</v>
       </c>
-      <c r="B19" t="s">
-        <v>155</v>
-      </c>
-      <c r="C19" t="s">
-        <v>156</v>
-      </c>
       <c r="E19" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B20" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C20" t="s">
+        <v>156</v>
+      </c>
+      <c r="E20" t="s">
         <v>158</v>
-      </c>
-      <c r="E20" t="s">
-        <v>160</v>
       </c>
     </row>
   </sheetData>
@@ -2327,21 +2327,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100396ED2E7A640164CB8C59FDEC2C765CC" ma:contentTypeVersion="8" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="26e8590940edae28bea0b080f6fa8b06">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="aceb4bc4-7be6-4130-8e8a-7008d72bfcc3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7a9331905dac936d9e88b896f6b901d6" ns3:_="">
     <xsd:import namespace="aceb4bc4-7be6-4130-8e8a-7008d72bfcc3"/>
@@ -2511,10 +2496,35 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{49E57FCB-AF0B-40B5-9F88-8BBFA3B90FEE}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E8D080FC-E009-4447-ACD6-B9CB0ED3D7DD}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="aceb4bc4-7be6-4130-8e8a-7008d72bfcc3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2536,19 +2546,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E8D080FC-E009-4447-ACD6-B9CB0ED3D7DD}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{49E57FCB-AF0B-40B5-9F88-8BBFA3B90FEE}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="aceb4bc4-7be6-4130-8e8a-7008d72bfcc3"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>